<commit_message>
Debugged more and updated README
</commit_message>
<xml_diff>
--- a/data/OfficerList.xlsx
+++ b/data/OfficerList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeyo\SC2002-Group-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7707600-1689-4FE1-8811-F126CC2204F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48CA047-1229-4CDB-812F-888E56ADCBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>Jobless</t>
   </si>
   <si>
-    <t>Primary School student</t>
-  </si>
-  <si>
     <t>T9574576H</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>T1918537J</t>
+  </si>
+  <si>
+    <t>Primary School Student</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -500,7 +500,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>31</v>
@@ -514,10 +514,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>10</v>

</xml_diff>